<commit_message>
Ya se acabó el tiempo :(
</commit_message>
<xml_diff>
--- a/docs/ModeloRelacional.xlsx
+++ b/docs/ModeloRelacional.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CAMILO\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CAMILO\Desktop\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE49CBE-B4D9-4261-A148-B84FC755B1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED0741F-A3D5-4CE4-8B81-3AA89051A972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Proyecto 1" sheetId="1" r:id="rId1"/>

</xml_diff>